<commit_message>
Updated requirements and Risk list
</commit_message>
<xml_diff>
--- a/Documentation/Risk_List.xlsx
+++ b/Documentation/Risk_List.xlsx
@@ -1,35 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\brdsb\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D98913A-172B-4F6C-AE06-703C386E7568}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
     <sheet name="Risk_Tracking_Log" sheetId="2" r:id="rId2"/>
     <sheet name="DropDown_Elements" sheetId="4" state="hidden" r:id="rId3"/>
+    <sheet name="Priority" sheetId="5" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Instructions!$A$24:$B$34</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Risk_Tracking_Log!$B$6:$D$6</definedName>
     <definedName name="as">[1]DropDown_Elements!$A$2:$A$30</definedName>
     <definedName name="OLE_LINK1" localSheetId="1">Risk_Tracking_Log!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Risk_Tracking_Log!$A$1:$M$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Risk_Tracking_Log!$A$1:$N$30</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Risk_Tracking_Log!$1:$6</definedName>
     <definedName name="Risk_Area">DropDown_Elements!$A$2:$A$30</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -41,13 +36,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>eze3</author>
     <author>e</author>
   </authors>
   <commentList>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="A6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -70,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="B6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -132,7 +127,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="C6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -215,7 +210,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="D6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -297,7 +292,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
+    <comment ref="E6" authorId="1">
       <text>
         <r>
           <rPr>
@@ -380,7 +375,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
+    <comment ref="F6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -403,7 +398,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
+    <comment ref="G6" authorId="1">
       <text>
         <r>
           <rPr>
@@ -425,7 +420,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
+    <comment ref="H6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -447,7 +442,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
+    <comment ref="I6" authorId="1">
       <text>
         <r>
           <rPr>
@@ -469,7 +464,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
+    <comment ref="J6" authorId="1">
       <text>
         <r>
           <rPr>
@@ -491,7 +486,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000B000000}">
+    <comment ref="K6" authorId="1">
       <text>
         <r>
           <rPr>
@@ -513,7 +508,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000C000000}">
+    <comment ref="L6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -536,7 +531,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000D000000}">
+    <comment ref="N6" authorId="1">
       <text>
         <r>
           <rPr>
@@ -563,7 +558,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="197">
   <si>
     <t>ID</t>
   </si>
@@ -1469,11 +1464,23 @@
   <si>
     <t>Chosen technology stack has a too high cost to implement when standing up final product. This would mean that the final product cannot be delivered to the client or provide the services expected, making the project a failure. Investigating and identifying appropriate hosting solutions is therefore a neccesary part of the planning phase of this project in order to avoid this.</t>
   </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
@@ -1600,7 +1607,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -2056,11 +2063,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2302,14 +2322,29 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="13" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2774,14 +2809,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2796,11 +2831,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="str">
+      <c r="A1" s="84" t="str">
         <f>Risk_Tracking_Log!A1</f>
         <v>RISK MANAGEMENT LOG</v>
       </c>
-      <c r="B1" s="84"/>
+      <c r="B1" s="85"/>
     </row>
     <row r="2" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="74" t="s">
@@ -2973,11 +3008,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:U30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2991,13 +3026,13 @@
     <col min="8" max="8" width="22.140625" style="48" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="30.85546875" style="48" customWidth="1"/>
     <col min="11" max="11" width="12.85546875" style="48" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="30.85546875" style="48" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="4"/>
-    <col min="15" max="15" width="6" style="4" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="4"/>
+    <col min="12" max="14" width="30.85546875" style="48" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="4"/>
+    <col min="16" max="16" width="6" style="4" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="7" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="7" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -3015,8 +3050,9 @@
       <c r="K1" s="30"/>
       <c r="L1" s="30"/>
       <c r="M1" s="30"/>
-    </row>
-    <row r="2" spans="1:21" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="N1" s="30"/>
+    </row>
+    <row r="2" spans="1:22" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>6</v>
       </c>
@@ -3048,8 +3084,9 @@
       <c r="S2" s="65"/>
       <c r="T2" s="65"/>
       <c r="U2" s="65"/>
-    </row>
-    <row r="3" spans="1:21" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="V2" s="65"/>
+    </row>
+    <row r="3" spans="1:22" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>77</v>
       </c>
@@ -3081,8 +3118,9 @@
       <c r="S3" s="65"/>
       <c r="T3" s="65"/>
       <c r="U3" s="65"/>
-    </row>
-    <row r="4" spans="1:21" s="1" customFormat="1" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="V3" s="65"/>
+    </row>
+    <row r="4" spans="1:22" s="1" customFormat="1" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -3114,14 +3152,15 @@
       <c r="S4" s="65"/>
       <c r="T4" s="65"/>
       <c r="U4" s="65"/>
-    </row>
-    <row r="5" spans="1:21" s="1" customFormat="1" ht="57" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="V4" s="65"/>
+    </row>
+    <row r="5" spans="1:22" s="1" customFormat="1" ht="57" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="31"/>
       <c r="C5" s="40"/>
-      <c r="D5" s="85" t="s">
+      <c r="D5" s="83" t="s">
         <v>162</v>
       </c>
       <c r="E5" s="51"/>
@@ -3138,8 +3177,8 @@
       </c>
       <c r="K5" s="51"/>
       <c r="L5" s="51"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="65"/>
+      <c r="M5" s="51"/>
+      <c r="N5" s="52"/>
       <c r="O5" s="65"/>
       <c r="P5" s="65"/>
       <c r="Q5" s="65"/>
@@ -3147,8 +3186,9 @@
       <c r="S5" s="65"/>
       <c r="T5" s="65"/>
       <c r="U5" s="65"/>
-    </row>
-    <row r="6" spans="1:21" s="3" customFormat="1" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="V5" s="65"/>
+    </row>
+    <row r="6" spans="1:22" s="3" customFormat="1" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="54" t="s">
         <v>0</v>
       </c>
@@ -3185,11 +3225,14 @@
       <c r="L6" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="M6" s="64" t="s">
+      <c r="M6" s="86" t="s">
+        <v>193</v>
+      </c>
+      <c r="N6" s="64" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" ht="78.75" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>85</v>
       </c>
@@ -3227,11 +3270,14 @@
       <c r="L7" s="79" t="s">
         <v>83</v>
       </c>
-      <c r="M7" s="80" t="s">
+      <c r="M7" s="87" t="s">
+        <v>3</v>
+      </c>
+      <c r="N7" s="80" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="101.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" ht="101.25" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>163</v>
       </c>
@@ -3269,11 +3315,14 @@
       <c r="L8" s="81" t="s">
         <v>103</v>
       </c>
-      <c r="M8" s="44" t="s">
+      <c r="M8" s="88" t="s">
+        <v>3</v>
+      </c>
+      <c r="N8" s="44" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="112.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" ht="112.5" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>164</v>
       </c>
@@ -3311,11 +3360,14 @@
       <c r="L9" s="78" t="s">
         <v>178</v>
       </c>
-      <c r="M9" s="45" t="s">
+      <c r="M9" s="89" t="s">
+        <v>3</v>
+      </c>
+      <c r="N9" s="45" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="146.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" ht="146.25" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>165</v>
       </c>
@@ -3353,11 +3405,14 @@
       <c r="L10" s="78" t="s">
         <v>176</v>
       </c>
-      <c r="M10" s="45" t="s">
+      <c r="M10" s="89" t="s">
+        <v>1</v>
+      </c>
+      <c r="N10" s="45" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="123.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" ht="123.75" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>166</v>
       </c>
@@ -3395,11 +3450,14 @@
       <c r="L11" s="78" t="s">
         <v>116</v>
       </c>
-      <c r="M11" s="45" t="s">
+      <c r="M11" s="89" t="s">
+        <v>194</v>
+      </c>
+      <c r="N11" s="45" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="146.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" ht="146.25" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>167</v>
       </c>
@@ -3437,11 +3495,14 @@
       <c r="L12" s="78" t="s">
         <v>147</v>
       </c>
-      <c r="M12" s="45" t="s">
+      <c r="M12" s="89" t="s">
+        <v>194</v>
+      </c>
+      <c r="N12" s="45" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="157.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" ht="157.5" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>168</v>
       </c>
@@ -3479,11 +3540,14 @@
       <c r="L13" s="78" t="s">
         <v>148</v>
       </c>
-      <c r="M13" s="45" t="s">
+      <c r="M13" s="89" t="s">
+        <v>194</v>
+      </c>
+      <c r="N13" s="45" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="123.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" ht="123.75" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>169</v>
       </c>
@@ -3521,11 +3585,14 @@
       <c r="L14" s="78" t="s">
         <v>150</v>
       </c>
-      <c r="M14" s="45" t="s">
+      <c r="M14" s="89" t="s">
+        <v>195</v>
+      </c>
+      <c r="N14" s="45" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" ht="78.75" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>170</v>
       </c>
@@ -3563,11 +3630,14 @@
       <c r="L15" s="78" t="s">
         <v>152</v>
       </c>
-      <c r="M15" s="45" t="s">
+      <c r="M15" s="89" t="s">
+        <v>196</v>
+      </c>
+      <c r="N15" s="45" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="90" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" ht="90" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>171</v>
       </c>
@@ -3605,11 +3675,14 @@
       <c r="L16" s="78" t="s">
         <v>152</v>
       </c>
-      <c r="M16" s="45" t="s">
+      <c r="M16" s="89" t="s">
+        <v>196</v>
+      </c>
+      <c r="N16" s="45" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="112.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" ht="112.5" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>172</v>
       </c>
@@ -3647,11 +3720,14 @@
       <c r="L17" s="78" t="s">
         <v>154</v>
       </c>
-      <c r="M17" s="45" t="s">
+      <c r="M17" s="89" t="s">
+        <v>194</v>
+      </c>
+      <c r="N17" s="45" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="90" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" ht="90" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>173</v>
       </c>
@@ -3689,11 +3765,14 @@
       <c r="L18" s="78" t="s">
         <v>156</v>
       </c>
-      <c r="M18" s="45" t="s">
+      <c r="M18" s="89" t="s">
+        <v>194</v>
+      </c>
+      <c r="N18" s="45" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="123.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="123.75" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>174</v>
       </c>
@@ -3731,11 +3810,14 @@
       <c r="L19" s="78" t="s">
         <v>158</v>
       </c>
-      <c r="M19" s="45" t="s">
+      <c r="M19" s="89" t="s">
+        <v>196</v>
+      </c>
+      <c r="N19" s="45" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="101.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="101.25" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>175</v>
       </c>
@@ -3773,11 +3855,14 @@
       <c r="L20" s="78" t="s">
         <v>184</v>
       </c>
-      <c r="M20" s="45" t="s">
+      <c r="M20" s="89" t="s">
+        <v>3</v>
+      </c>
+      <c r="N20" s="45" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="123.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" ht="123.75" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>185</v>
       </c>
@@ -3815,11 +3900,14 @@
       <c r="L21" s="78" t="s">
         <v>190</v>
       </c>
-      <c r="M21" s="45" t="s">
+      <c r="M21" s="89" t="s">
+        <v>196</v>
+      </c>
+      <c r="N21" s="45" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="12"/>
       <c r="B22" s="14"/>
       <c r="C22" s="27"/>
@@ -3835,9 +3923,10 @@
       <c r="J22" s="62"/>
       <c r="K22" s="72"/>
       <c r="L22" s="78"/>
-      <c r="M22" s="45"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M22" s="89"/>
+      <c r="N22" s="45"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="12"/>
       <c r="B23" s="14"/>
       <c r="C23" s="27"/>
@@ -3853,9 +3942,10 @@
       <c r="J23" s="62"/>
       <c r="K23" s="72"/>
       <c r="L23" s="78"/>
-      <c r="M23" s="45"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M23" s="89"/>
+      <c r="N23" s="45"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="12"/>
       <c r="B24" s="14"/>
       <c r="C24" s="27"/>
@@ -3871,9 +3961,10 @@
       <c r="J24" s="62"/>
       <c r="K24" s="72"/>
       <c r="L24" s="78"/>
-      <c r="M24" s="45"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M24" s="89"/>
+      <c r="N24" s="45"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="12"/>
       <c r="B25" s="14"/>
       <c r="C25" s="27"/>
@@ -3889,9 +3980,10 @@
       <c r="J25" s="62"/>
       <c r="K25" s="72"/>
       <c r="L25" s="78"/>
-      <c r="M25" s="45"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M25" s="89"/>
+      <c r="N25" s="45"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="12"/>
       <c r="B26" s="14"/>
       <c r="C26" s="27"/>
@@ -3907,9 +3999,10 @@
       <c r="J26" s="62"/>
       <c r="K26" s="72"/>
       <c r="L26" s="78"/>
-      <c r="M26" s="45"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M26" s="89"/>
+      <c r="N26" s="45"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="12"/>
       <c r="B27" s="14"/>
       <c r="C27" s="27"/>
@@ -3925,9 +4018,10 @@
       <c r="J27" s="62"/>
       <c r="K27" s="72"/>
       <c r="L27" s="78"/>
-      <c r="M27" s="45"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M27" s="89"/>
+      <c r="N27" s="45"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="12"/>
       <c r="B28" s="14"/>
       <c r="C28" s="27"/>
@@ -3943,9 +4037,10 @@
       <c r="J28" s="62"/>
       <c r="K28" s="72"/>
       <c r="L28" s="78"/>
-      <c r="M28" s="45"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M28" s="89"/>
+      <c r="N28" s="45"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="12"/>
       <c r="B29" s="14"/>
       <c r="C29" s="27"/>
@@ -3961,9 +4056,10 @@
       <c r="J29" s="62"/>
       <c r="K29" s="72"/>
       <c r="L29" s="78"/>
-      <c r="M29" s="45"/>
-    </row>
-    <row r="30" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M29" s="89"/>
+      <c r="N29" s="45"/>
+    </row>
+    <row r="30" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="15"/>
       <c r="C30" s="59"/>
@@ -3979,10 +4075,11 @@
       <c r="J30" s="69"/>
       <c r="K30" s="71"/>
       <c r="L30" s="82"/>
-      <c r="M30" s="47"/>
+      <c r="M30" s="90"/>
+      <c r="N30" s="47"/>
     </row>
   </sheetData>
-  <autoFilter ref="B6:D6" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="B6:D6"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="C31:E65531 C1:E1 B6:C6 B7:B30">
     <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">
@@ -3995,7 +4092,7 @@
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L7:L30">
+  <conditionalFormatting sqref="L7:M30">
     <cfRule type="cellIs" dxfId="7" priority="4" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
@@ -4026,16 +4123,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:D30" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:D30">
       <formula1>"High,Medium,Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H30" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H30">
       <formula1>Risk_Area</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B30" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B30">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7:K30" xr:uid="{00000000-0002-0000-0100-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7:K30">
       <formula1>"Acceptance,Avoidance,Contingency,Mitigation,Transfer"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4049,7 +4146,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4166,4 +4263,16 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>